<commit_message>
Add cultivar names into obs file so can filter them
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/data/Lincoln2024.xlsx
+++ b/Tests/Validation/Wheat/data/Lincoln2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0EF73D-E86A-4346-82AB-877875FC482E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C414218D-CF13-438C-9A2C-7D5427A1FDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" autoFilterDateGrouping="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1850" uniqueCount="74">
   <si>
     <t>SimulationName</t>
   </si>
@@ -321,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -339,6 +339,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -675,13 +678,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y1549"/>
+  <dimension ref="A1:Y1593"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="R826" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G1583" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R834" sqref="R834:R837"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,7 +697,8 @@
     <col min="6" max="6" width="24" customWidth="1"/>
     <col min="7" max="7" width="25.33203125" customWidth="1"/>
     <col min="8" max="16" width="23.6640625" customWidth="1"/>
-    <col min="17" max="19" width="36.33203125" customWidth="1"/>
+    <col min="17" max="18" width="36.33203125" customWidth="1"/>
+    <col min="19" max="19" width="21.21875" customWidth="1"/>
     <col min="20" max="20" width="22.5546875" customWidth="1"/>
     <col min="21" max="21" width="19.6640625" customWidth="1"/>
     <col min="22" max="22" width="17.6640625" customWidth="1"/>
@@ -22309,6 +22313,886 @@
       </c>
       <c r="Y1549">
         <v>6.416666666666667</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1550" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1550" s="12">
+        <v>45597</v>
+      </c>
+      <c r="D1550">
+        <v>278.87147971955255</v>
+      </c>
+      <c r="E1550">
+        <v>1602.0306076560514</v>
+      </c>
+      <c r="F1550">
+        <v>125.43580675659413</v>
+      </c>
+      <c r="I1550">
+        <v>286.34333848191739</v>
+      </c>
+    </row>
+    <row r="1551" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1551" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1551" s="1">
+        <v>45604</v>
+      </c>
+      <c r="D1551">
+        <v>282.86709376756733</v>
+      </c>
+      <c r="E1551">
+        <v>1842.6067734508706</v>
+      </c>
+      <c r="F1551">
+        <v>135.72798551076588</v>
+      </c>
+      <c r="I1551">
+        <v>372.39088572637337</v>
+      </c>
+    </row>
+    <row r="1552" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1552" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1552" s="1">
+        <v>45610</v>
+      </c>
+      <c r="D1552">
+        <v>208.95687521286453</v>
+      </c>
+      <c r="E1552">
+        <v>1776.6500658526024</v>
+      </c>
+      <c r="F1552">
+        <v>155.42244509321344</v>
+      </c>
+      <c r="I1552">
+        <v>433.2691712777081</v>
+      </c>
+    </row>
+    <row r="1553" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1553" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1553" s="1">
+        <v>45618</v>
+      </c>
+      <c r="D1553">
+        <v>204.1123438524767</v>
+      </c>
+      <c r="E1553">
+        <v>1817.9819728730499</v>
+      </c>
+      <c r="F1553">
+        <v>153.6704579186657</v>
+      </c>
+      <c r="I1553">
+        <v>668.97705054486369</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1554" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1554" s="1">
+        <v>45625</v>
+      </c>
+      <c r="D1554">
+        <v>243.62531043507965</v>
+      </c>
+      <c r="E1554">
+        <v>2035.5619663141672</v>
+      </c>
+      <c r="F1554">
+        <v>180.83901074198857</v>
+      </c>
+      <c r="I1554">
+        <v>1016.9246704628633</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1555" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1555" s="1">
+        <v>45631</v>
+      </c>
+      <c r="D1555">
+        <v>136.99459356932547</v>
+      </c>
+      <c r="E1555">
+        <v>1630.3612142051293</v>
+      </c>
+      <c r="F1555">
+        <v>251.64752591679314</v>
+      </c>
+      <c r="I1555">
+        <v>1358.9315943449826</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1556" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1556" s="1">
+        <v>45637</v>
+      </c>
+      <c r="D1556">
+        <v>108.39265189252511</v>
+      </c>
+      <c r="E1556">
+        <v>1501.8429227893459</v>
+      </c>
+      <c r="F1556">
+        <v>268.45482460901212</v>
+      </c>
+      <c r="I1556">
+        <v>1767.7930397256848</v>
+      </c>
+    </row>
+    <row r="1557" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1557" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1557" s="1">
+        <v>45644</v>
+      </c>
+      <c r="D1557">
+        <v>85.444857315520778</v>
+      </c>
+      <c r="E1557">
+        <v>1335.0393608785985</v>
+      </c>
+      <c r="F1557">
+        <v>258.13673000364884</v>
+      </c>
+      <c r="I1557">
+        <v>2148.2317297268428</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1558" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1558" s="1">
+        <v>45650</v>
+      </c>
+      <c r="D1558">
+        <v>13.123665047468437</v>
+      </c>
+      <c r="E1558">
+        <v>1260.9441667998744</v>
+      </c>
+      <c r="F1558">
+        <v>341.68168626063994</v>
+      </c>
+      <c r="I1558">
+        <v>2417.6854251560671</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1559" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1559" s="1">
+        <v>45656</v>
+      </c>
+      <c r="D1559">
+        <v>0</v>
+      </c>
+      <c r="E1559">
+        <v>1100.7334204888077</v>
+      </c>
+      <c r="F1559">
+        <v>370.37609199170265</v>
+      </c>
+      <c r="I1559">
+        <v>2360.9013202179913</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1560" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1560" s="1">
+        <v>45663</v>
+      </c>
+      <c r="D1560">
+        <v>0</v>
+      </c>
+      <c r="E1560">
+        <v>1015.7814467292733</v>
+      </c>
+      <c r="F1560">
+        <v>294.70490602526115</v>
+      </c>
+      <c r="I1560">
+        <v>2086.1607786148975</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1561" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1561" s="1">
+        <v>45597</v>
+      </c>
+      <c r="D1561">
+        <v>449.06310448489069</v>
+      </c>
+      <c r="E1561">
+        <v>1863.8409604973463</v>
+      </c>
+      <c r="F1561">
+        <v>112.89645620236203</v>
+      </c>
+      <c r="I1561">
+        <v>329.69429380908326</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1562" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1562" s="1">
+        <v>45604</v>
+      </c>
+      <c r="D1562">
+        <v>408.88193953844853</v>
+      </c>
+      <c r="E1562">
+        <v>1776.710706619858</v>
+      </c>
+      <c r="F1562">
+        <v>102.95759727412306</v>
+      </c>
+      <c r="I1562">
+        <v>374.82335583862925</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1563" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1563" s="1">
+        <v>45610</v>
+      </c>
+      <c r="D1563">
+        <v>338.10726437090386</v>
+      </c>
+      <c r="E1563">
+        <v>2056.7109163546615</v>
+      </c>
+      <c r="F1563">
+        <v>127.76178655901568</v>
+      </c>
+      <c r="I1563">
+        <v>474.46898821776767</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1564" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1564" s="1">
+        <v>45618</v>
+      </c>
+      <c r="D1564">
+        <v>373.13635477443734</v>
+      </c>
+      <c r="E1564">
+        <v>2082.3687585393864</v>
+      </c>
+      <c r="F1564">
+        <v>104.71738647306412</v>
+      </c>
+      <c r="I1564">
+        <v>691.00767781564412</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1565" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1565" s="1">
+        <v>45625</v>
+      </c>
+      <c r="D1565">
+        <v>316.75768574125851</v>
+      </c>
+      <c r="E1565">
+        <v>2145.4009574182942</v>
+      </c>
+      <c r="F1565">
+        <v>189.98158021266462</v>
+      </c>
+      <c r="I1565">
+        <v>1130.1191945026715</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1566" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1566" s="1">
+        <v>45631</v>
+      </c>
+      <c r="D1566">
+        <v>294.11281369955356</v>
+      </c>
+      <c r="E1566">
+        <v>2041.2841052921665</v>
+      </c>
+      <c r="F1566">
+        <v>181.23353208103296</v>
+      </c>
+      <c r="I1566">
+        <v>1514.4728834719642</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1567" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1567" s="1">
+        <v>45637</v>
+      </c>
+      <c r="D1567">
+        <v>258.28823302104024</v>
+      </c>
+      <c r="E1567">
+        <v>1827.4344542916051</v>
+      </c>
+      <c r="F1567">
+        <v>227.7889565165284</v>
+      </c>
+      <c r="I1567">
+        <v>1895.3564896875487</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1568" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1568" s="1">
+        <v>45644</v>
+      </c>
+      <c r="D1568">
+        <v>220.72429200967147</v>
+      </c>
+      <c r="E1568">
+        <v>1549.7556732010034</v>
+      </c>
+      <c r="F1568">
+        <v>201.22701023133186</v>
+      </c>
+      <c r="I1568">
+        <v>2451.277432217395</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1569" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1569" s="1">
+        <v>45650</v>
+      </c>
+      <c r="D1569">
+        <v>91.043943931492464</v>
+      </c>
+      <c r="E1569">
+        <v>1390.3038194136948</v>
+      </c>
+      <c r="F1569">
+        <v>300.67488131047168</v>
+      </c>
+      <c r="I1569">
+        <v>2675.9253562720319</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1570" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1570" s="1">
+        <v>45656</v>
+      </c>
+      <c r="D1570">
+        <v>61.988216464843276</v>
+      </c>
+      <c r="E1570">
+        <v>1288.0779880136479</v>
+      </c>
+      <c r="F1570">
+        <v>327.61268603122437</v>
+      </c>
+      <c r="I1570">
+        <v>2909.0410933907701</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1571" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1571" s="1">
+        <v>45663</v>
+      </c>
+      <c r="D1571">
+        <v>16.678329944359628</v>
+      </c>
+      <c r="E1571">
+        <v>1193.6529923653559</v>
+      </c>
+      <c r="F1571">
+        <v>317.04178865183826</v>
+      </c>
+      <c r="I1571">
+        <v>2486.9908485024071</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1572" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1572" s="1">
+        <v>45597</v>
+      </c>
+      <c r="D1572">
+        <v>415.22016874701114</v>
+      </c>
+      <c r="E1572">
+        <v>1600.385730890262</v>
+      </c>
+      <c r="F1572">
+        <v>132.98844733685718</v>
+      </c>
+      <c r="I1572">
+        <v>277.42532970992147</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1573" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1573" s="1">
+        <v>45604</v>
+      </c>
+      <c r="D1573">
+        <v>446.67035476974218</v>
+      </c>
+      <c r="E1573">
+        <v>1769.1736306968644</v>
+      </c>
+      <c r="F1573">
+        <v>152.22275917420157</v>
+      </c>
+      <c r="I1573">
+        <v>397.820234643189</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1574" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1574" s="1">
+        <v>45610</v>
+      </c>
+      <c r="D1574">
+        <v>426.3562140813932</v>
+      </c>
+      <c r="E1574">
+        <v>1695.1513781097215</v>
+      </c>
+      <c r="F1574">
+        <v>102.50855144462201</v>
+      </c>
+      <c r="I1574">
+        <v>439.69822603225236</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1575" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1575" s="1">
+        <v>45618</v>
+      </c>
+      <c r="D1575">
+        <v>393.47926553917034</v>
+      </c>
+      <c r="E1575">
+        <v>1979.801940795033</v>
+      </c>
+      <c r="F1575">
+        <v>157.69280794493309</v>
+      </c>
+      <c r="I1575">
+        <v>733.76253763854754</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1576" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1576" s="1">
+        <v>45625</v>
+      </c>
+      <c r="D1576">
+        <v>438.17891064379398</v>
+      </c>
+      <c r="E1576">
+        <v>2215.361621881571</v>
+      </c>
+      <c r="F1576">
+        <v>150.57108174240977</v>
+      </c>
+      <c r="I1576">
+        <v>1189.4543229336527</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1577" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1577" s="1">
+        <v>45631</v>
+      </c>
+      <c r="D1577">
+        <v>446.11715325474518</v>
+      </c>
+      <c r="E1577">
+        <v>2246.572820744213</v>
+      </c>
+      <c r="F1577">
+        <v>171.02298734068302</v>
+      </c>
+      <c r="I1577">
+        <v>1639.9361318887552</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1578" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1578" s="1">
+        <v>45637</v>
+      </c>
+      <c r="D1578">
+        <v>309.45394979689769</v>
+      </c>
+      <c r="E1578">
+        <v>1889.405858311271</v>
+      </c>
+      <c r="F1578">
+        <v>210.89403009268602</v>
+      </c>
+      <c r="I1578">
+        <v>1954.0972950304247</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1579" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1579" s="1">
+        <v>45644</v>
+      </c>
+      <c r="D1579">
+        <v>266.07289423895742</v>
+      </c>
+      <c r="E1579">
+        <v>1554.5976625938974</v>
+      </c>
+      <c r="F1579">
+        <v>247.24567850519992</v>
+      </c>
+      <c r="I1579">
+        <v>2333.9275296536803</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1580" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1580" s="1">
+        <v>45650</v>
+      </c>
+      <c r="D1580">
+        <v>102.73555771562553</v>
+      </c>
+      <c r="E1580">
+        <v>1577.883375463912</v>
+      </c>
+      <c r="F1580">
+        <v>345.74726369035983</v>
+      </c>
+      <c r="I1580">
+        <v>3035.3261120304801</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1581" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1581" s="1">
+        <v>45656</v>
+      </c>
+      <c r="D1581">
+        <v>88.431849729217817</v>
+      </c>
+      <c r="E1581">
+        <v>1445.8538223815892</v>
+      </c>
+      <c r="F1581">
+        <v>339.20551859734059</v>
+      </c>
+      <c r="I1581">
+        <v>3255.4777084854377</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1582" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1582" s="1">
+        <v>45663</v>
+      </c>
+      <c r="D1582">
+        <v>0</v>
+      </c>
+      <c r="E1582">
+        <v>1398.3231445323981</v>
+      </c>
+      <c r="F1582">
+        <v>354.499341548953</v>
+      </c>
+      <c r="I1582">
+        <v>2798.0237715363896</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1583" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1583" s="1">
+        <v>45597</v>
+      </c>
+      <c r="D1583">
+        <v>494.40043935304925</v>
+      </c>
+      <c r="E1583">
+        <v>1693.6091392008793</v>
+      </c>
+      <c r="F1583">
+        <v>86.864936950205049</v>
+      </c>
+      <c r="I1583">
+        <v>356.6092829408928</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1584" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1584" s="1">
+        <v>45604</v>
+      </c>
+      <c r="D1584">
+        <v>503.62896006171928</v>
+      </c>
+      <c r="E1584">
+        <v>1910.8711873026075</v>
+      </c>
+      <c r="F1584">
+        <v>111.64829048218641</v>
+      </c>
+      <c r="I1584">
+        <v>450.13517961230821</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1585" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1585" s="1">
+        <v>45610</v>
+      </c>
+      <c r="D1585">
+        <v>500.85046265495754</v>
+      </c>
+      <c r="E1585">
+        <v>2107.6276434466245</v>
+      </c>
+      <c r="F1585">
+        <v>117.2187949004025</v>
+      </c>
+      <c r="I1585">
+        <v>552.17583026562102</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1586" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1586" s="1">
+        <v>45618</v>
+      </c>
+      <c r="D1586">
+        <v>426.65396343069091</v>
+      </c>
+      <c r="E1586">
+        <v>2092.8185613616679</v>
+      </c>
+      <c r="F1586">
+        <v>140.95655355875937</v>
+      </c>
+      <c r="I1586">
+        <v>788.24226538281823</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1587" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1587" s="1">
+        <v>45625</v>
+      </c>
+      <c r="D1587">
+        <v>450.21651520831301</v>
+      </c>
+      <c r="E1587">
+        <v>2210.4525326468183</v>
+      </c>
+      <c r="F1587">
+        <v>179.8960162650242</v>
+      </c>
+      <c r="I1587">
+        <v>1202.80589909276</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1588" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1588" s="1">
+        <v>45631</v>
+      </c>
+      <c r="D1588">
+        <v>409.95245869881114</v>
+      </c>
+      <c r="E1588">
+        <v>2181.5429988675255</v>
+      </c>
+      <c r="F1588">
+        <v>191.18178753622394</v>
+      </c>
+      <c r="I1588">
+        <v>1704.7244335422038</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1589" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1589" s="1">
+        <v>45637</v>
+      </c>
+      <c r="D1589">
+        <v>314.65142427886246</v>
+      </c>
+      <c r="E1589">
+        <v>1787.5591050714811</v>
+      </c>
+      <c r="F1589">
+        <v>227.06282818460437</v>
+      </c>
+      <c r="I1589">
+        <v>1995.0810911222779</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1590" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1590" s="1">
+        <v>45644</v>
+      </c>
+      <c r="D1590">
+        <v>261.38595695602095</v>
+      </c>
+      <c r="E1590">
+        <v>1560.2297313442755</v>
+      </c>
+      <c r="F1590">
+        <v>243.68975700023415</v>
+      </c>
+      <c r="I1590">
+        <v>2517.440328998674</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1591" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1591" s="1">
+        <v>45650</v>
+      </c>
+      <c r="D1591">
+        <v>264.71586785552631</v>
+      </c>
+      <c r="E1591">
+        <v>1567.7022895058094</v>
+      </c>
+      <c r="F1591">
+        <v>241.70789629313876</v>
+      </c>
+      <c r="I1591">
+        <v>3000.1469757147506</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1592" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1592" s="1">
+        <v>45656</v>
+      </c>
+      <c r="D1592">
+        <v>67.252714674168999</v>
+      </c>
+      <c r="E1592">
+        <v>1494.7710088968145</v>
+      </c>
+      <c r="F1592">
+        <v>377.82888366675627</v>
+      </c>
+      <c r="I1592">
+        <v>3198.991507884336</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1593" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1593" s="1">
+        <v>45663</v>
+      </c>
+      <c r="D1593">
+        <v>20.807004426980797</v>
+      </c>
+      <c r="E1593">
+        <v>1355.9054761598836</v>
+      </c>
+      <c r="F1593">
+        <v>370.5811826661656</v>
+      </c>
+      <c r="I1593">
+        <v>2785.8836981060431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove biomass derived from random stem samples
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/data/Lincoln2024.xlsx
+++ b/Tests/Validation/Wheat/data/Lincoln2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C414218D-CF13-438C-9A2C-7D5427A1FDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBED1540-ED72-4C5F-B083-F756F67104E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" autoFilterDateGrouping="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1850" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="75">
   <si>
     <t>SimulationName</t>
   </si>
@@ -262,6 +262,9 @@
   <si>
     <t>HarvestRipe</t>
   </si>
+  <si>
+    <t>DoubleRidge</t>
+  </si>
 </sst>
 </file>
 
@@ -294,7 +297,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,6 +307,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -340,9 +349,8 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,13 +686,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y1593"/>
+  <dimension ref="A1:Y1821"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G1583" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C1558" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="A1558" sqref="A1558:XFD1649"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,7 +713,7 @@
     <col min="23" max="23" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -22315,884 +22323,3020 @@
         <v>6.416666666666667</v>
       </c>
     </row>
-    <row r="1550" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1550" s="4" t="s">
+    <row r="1550" spans="1:25" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1550" s="13" t="s">
         <v>33</v>
       </c>
       <c r="B1550" s="12">
-        <v>45597</v>
-      </c>
-      <c r="D1550">
-        <v>278.87147971955255</v>
-      </c>
-      <c r="E1550">
-        <v>1602.0306076560514</v>
-      </c>
-      <c r="F1550">
-        <v>125.43580675659413</v>
-      </c>
-      <c r="I1550">
-        <v>286.34333848191739</v>
-      </c>
-    </row>
-    <row r="1551" spans="1:25" x14ac:dyDescent="0.3">
+        <v>45483</v>
+      </c>
+      <c r="R1550" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1550" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1551" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1551" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1551" s="1">
-        <v>45604</v>
-      </c>
-      <c r="D1551">
-        <v>282.86709376756733</v>
-      </c>
-      <c r="E1551">
-        <v>1842.6067734508706</v>
-      </c>
-      <c r="F1551">
-        <v>135.72798551076588</v>
-      </c>
-      <c r="I1551">
-        <v>372.39088572637337</v>
-      </c>
-    </row>
-    <row r="1552" spans="1:25" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="B1551" s="9">
+        <v>45483</v>
+      </c>
+      <c r="R1551" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1551">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1552" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1552" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1552" s="1">
-        <v>45610</v>
-      </c>
-      <c r="D1552">
-        <v>208.95687521286453</v>
-      </c>
-      <c r="E1552">
-        <v>1776.6500658526024</v>
-      </c>
-      <c r="F1552">
-        <v>155.42244509321344</v>
-      </c>
-      <c r="I1552">
-        <v>433.2691712777081</v>
-      </c>
-    </row>
-    <row r="1553" spans="1:9" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="B1552" s="9">
+        <v>45483</v>
+      </c>
+      <c r="R1552" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1552">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1553" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1553" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1553" s="1">
-        <v>45618</v>
-      </c>
-      <c r="D1553">
-        <v>204.1123438524767</v>
-      </c>
-      <c r="E1553">
-        <v>1817.9819728730499</v>
-      </c>
-      <c r="F1553">
-        <v>153.6704579186657</v>
-      </c>
-      <c r="I1553">
-        <v>668.97705054486369</v>
-      </c>
-    </row>
-    <row r="1554" spans="1:9" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="B1553" s="9">
+        <v>45483</v>
+      </c>
+      <c r="R1553" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1553">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1554" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1554" s="1">
-        <v>45625</v>
-      </c>
-      <c r="D1554">
-        <v>243.62531043507965</v>
-      </c>
-      <c r="E1554">
-        <v>2035.5619663141672</v>
-      </c>
-      <c r="F1554">
-        <v>180.83901074198857</v>
-      </c>
-      <c r="I1554">
-        <v>1016.9246704628633</v>
-      </c>
-    </row>
-    <row r="1555" spans="1:9" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="B1554" s="9">
+        <v>45527</v>
+      </c>
+      <c r="R1554" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1554">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1555" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1555" s="1">
-        <v>45631</v>
-      </c>
-      <c r="D1555">
-        <v>136.99459356932547</v>
-      </c>
-      <c r="E1555">
-        <v>1630.3612142051293</v>
-      </c>
-      <c r="F1555">
-        <v>251.64752591679314</v>
-      </c>
-      <c r="I1555">
-        <v>1358.9315943449826</v>
-      </c>
-    </row>
-    <row r="1556" spans="1:9" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="B1555" s="9">
+        <v>45527</v>
+      </c>
+      <c r="R1555" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1555">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1556" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1556" s="1">
-        <v>45637</v>
-      </c>
-      <c r="D1556">
-        <v>108.39265189252511</v>
-      </c>
-      <c r="E1556">
-        <v>1501.8429227893459</v>
-      </c>
-      <c r="F1556">
-        <v>268.45482460901212</v>
-      </c>
-      <c r="I1556">
-        <v>1767.7930397256848</v>
-      </c>
-    </row>
-    <row r="1557" spans="1:9" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="B1556" s="9">
+        <v>45527</v>
+      </c>
+      <c r="R1556" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1556">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1557" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1557" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1557" s="1">
-        <v>45644</v>
-      </c>
-      <c r="D1557">
-        <v>85.444857315520778</v>
-      </c>
-      <c r="E1557">
-        <v>1335.0393608785985</v>
-      </c>
-      <c r="F1557">
-        <v>258.13673000364884</v>
-      </c>
-      <c r="I1557">
-        <v>2148.2317297268428</v>
-      </c>
-    </row>
-    <row r="1558" spans="1:9" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="B1557" s="9">
+        <v>45527</v>
+      </c>
+      <c r="R1557" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1557">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1558" t="s">
         <v>33</v>
       </c>
       <c r="B1558" s="1">
-        <v>45650</v>
-      </c>
-      <c r="D1558">
-        <v>13.123665047468437</v>
-      </c>
-      <c r="E1558">
-        <v>1260.9441667998744</v>
-      </c>
-      <c r="F1558">
-        <v>341.68168626063994</v>
-      </c>
-      <c r="I1558">
-        <v>2417.6854251560671</v>
-      </c>
-    </row>
-    <row r="1559" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45443</v>
+      </c>
+      <c r="Y1558">
+        <v>9.8333333333333321</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1559" t="s">
         <v>33</v>
       </c>
       <c r="B1559" s="1">
-        <v>45656</v>
-      </c>
-      <c r="D1559">
-        <v>0</v>
-      </c>
-      <c r="E1559">
-        <v>1100.7334204888077</v>
-      </c>
-      <c r="F1559">
-        <v>370.37609199170265</v>
-      </c>
-      <c r="I1559">
-        <v>2360.9013202179913</v>
-      </c>
-    </row>
-    <row r="1560" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45449</v>
+      </c>
+      <c r="Y1559">
+        <v>10.333333333333334</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1560" t="s">
         <v>33</v>
       </c>
       <c r="B1560" s="1">
+        <v>45456</v>
+      </c>
+      <c r="Y1560">
+        <v>15.666666666666666</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1561" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1561" s="1">
+        <v>45462</v>
+      </c>
+      <c r="Y1561">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1562" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1562" s="1">
+        <v>45469</v>
+      </c>
+      <c r="Y1562">
+        <v>19.833333333333336</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1563" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1563" s="1">
+        <v>45477</v>
+      </c>
+      <c r="Y1563">
+        <v>15.166666666666668</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1564" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1564" s="1">
+        <v>45483</v>
+      </c>
+      <c r="Y1564">
+        <v>20.166666666666668</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1565" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1565" s="1">
+        <v>45492</v>
+      </c>
+      <c r="Y1565">
+        <v>14.166666666666666</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1566" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1566" s="1">
+        <v>45500</v>
+      </c>
+      <c r="Y1566">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1567" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1567" s="1">
+        <v>45505</v>
+      </c>
+      <c r="Y1567">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1568" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1568" s="1">
+        <v>45512</v>
+      </c>
+      <c r="Y1568">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1569" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1569" s="1">
+        <v>45520</v>
+      </c>
+      <c r="Y1569">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1570" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1570" s="1">
+        <v>45527</v>
+      </c>
+      <c r="Y1570">
+        <v>16.166666666666668</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1571" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1571" s="1">
+        <v>45533</v>
+      </c>
+      <c r="Y1571">
+        <v>11.666666666666666</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1572" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1572" s="1">
+        <v>45539</v>
+      </c>
+      <c r="Y1572">
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1573" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1573" s="1">
+        <v>45545</v>
+      </c>
+      <c r="Y1573">
+        <v>9.3333333333333321</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1574" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1574" s="1">
+        <v>45555</v>
+      </c>
+      <c r="Y1574">
+        <v>9.1666666666666661</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1575" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1575" s="1">
+        <v>45562</v>
+      </c>
+      <c r="Y1575">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1576" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1576" s="1">
+        <v>45569</v>
+      </c>
+      <c r="Y1576">
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1577" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1577" s="1">
+        <v>45575</v>
+      </c>
+      <c r="Y1577">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1578" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1578" s="1">
+        <v>45581</v>
+      </c>
+      <c r="Y1578">
+        <v>8.1666666666666661</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1579" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1579" s="1">
+        <v>45590</v>
+      </c>
+      <c r="Y1579">
+        <v>8.1666666666666679</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1580" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1580" s="1">
+        <v>45597</v>
+      </c>
+      <c r="Y1580">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1581" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1581" s="1">
+        <v>45604</v>
+      </c>
+      <c r="Y1581">
+        <v>5.6666666666666661</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1582" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1582" s="1">
+        <v>45610</v>
+      </c>
+      <c r="Y1582">
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1583" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1583" s="1">
+        <v>45618</v>
+      </c>
+      <c r="Y1583">
+        <v>5.4791666666666661</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1584" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1584" s="1">
+        <v>45625</v>
+      </c>
+      <c r="Y1584">
+        <v>5.3333333333333339</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1585" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1585" s="1">
+        <v>45631</v>
+      </c>
+      <c r="Y1585">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1586" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1586" s="1">
+        <v>45637</v>
+      </c>
+      <c r="Y1586">
+        <v>5.083333333333333</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1587" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1587" s="1">
+        <v>45644</v>
+      </c>
+      <c r="Y1587">
+        <v>4.916666666666667</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1588" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1588" s="1">
+        <v>45650</v>
+      </c>
+      <c r="Y1588">
+        <v>4.4166666666666661</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1589" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1589" s="1">
+        <v>45656</v>
+      </c>
+      <c r="Y1589">
+        <v>4.3333333333333339</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1590" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1590" s="1">
         <v>45663</v>
       </c>
-      <c r="D1560">
-        <v>0</v>
-      </c>
-      <c r="E1560">
-        <v>1015.7814467292733</v>
-      </c>
-      <c r="F1560">
-        <v>294.70490602526115</v>
-      </c>
-      <c r="I1560">
-        <v>2086.1607786148975</v>
-      </c>
-    </row>
-    <row r="1561" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1561" t="s">
+      <c r="Y1590">
+        <v>4.333333333333333</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1591" t="s">
         <v>36</v>
       </c>
-      <c r="B1561" s="1">
+      <c r="B1591" s="1">
+        <v>45443</v>
+      </c>
+      <c r="Y1591">
+        <v>10.666666666666668</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1592" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1592" s="1">
+        <v>45449</v>
+      </c>
+      <c r="Y1592">
+        <v>12.833333333333332</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1593" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1593" s="1">
+        <v>45456</v>
+      </c>
+      <c r="Y1593">
+        <v>13.666666666666666</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1594" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1594" s="1">
+        <v>45462</v>
+      </c>
+      <c r="Y1594">
+        <v>15.833333333333332</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1595" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1595" s="1">
+        <v>45469</v>
+      </c>
+      <c r="Y1595">
+        <v>17.833333333333336</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1596" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1596" s="1">
+        <v>45477</v>
+      </c>
+      <c r="Y1596">
+        <v>15.833333333333332</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1597" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1597" s="1">
+        <v>45483</v>
+      </c>
+      <c r="Y1597">
+        <v>16.333333333333332</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1598" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1598" s="1">
+        <v>45492</v>
+      </c>
+      <c r="Y1598">
+        <v>14.166666666666666</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1599" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1599" s="1">
+        <v>45500</v>
+      </c>
+      <c r="Y1599">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1600" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1600" s="1">
+        <v>45505</v>
+      </c>
+      <c r="Y1600">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1601" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1601" s="1">
+        <v>45512</v>
+      </c>
+      <c r="Y1601">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1602" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1602" s="1">
+        <v>45520</v>
+      </c>
+      <c r="Y1602">
+        <v>17.166666666666664</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1603" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1603" s="1">
+        <v>45527</v>
+      </c>
+      <c r="Y1603">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1604" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1604" s="1">
+        <v>45533</v>
+      </c>
+      <c r="Y1604">
+        <v>16.666666666666664</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1605" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1605" s="1">
+        <v>45539</v>
+      </c>
+      <c r="Y1605">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1606" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1606" s="1">
+        <v>45545</v>
+      </c>
+      <c r="Y1606">
+        <v>12.833333333333334</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1607" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1607" s="1">
+        <v>45555</v>
+      </c>
+      <c r="Y1607">
+        <v>8.8333333333333339</v>
+      </c>
+    </row>
+    <row r="1608" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1608" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1608" s="1">
+        <v>45562</v>
+      </c>
+      <c r="Y1608">
+        <v>7.4583333333333339</v>
+      </c>
+    </row>
+    <row r="1609" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1609" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1609" s="1">
+        <v>45569</v>
+      </c>
+      <c r="Y1609">
+        <v>9.4166666666666679</v>
+      </c>
+    </row>
+    <row r="1610" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1610" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1610" s="1">
+        <v>45575</v>
+      </c>
+      <c r="Y1610">
+        <v>10.666666666666668</v>
+      </c>
+    </row>
+    <row r="1611" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1611" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1611" s="1">
+        <v>45581</v>
+      </c>
+      <c r="Y1611">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1612" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1612" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1612" s="1">
+        <v>45590</v>
+      </c>
+      <c r="Y1612">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="1613" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1613" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1613" s="1">
         <v>45597</v>
       </c>
-      <c r="D1561">
-        <v>449.06310448489069</v>
-      </c>
-      <c r="E1561">
-        <v>1863.8409604973463</v>
-      </c>
-      <c r="F1561">
-        <v>112.89645620236203</v>
-      </c>
-      <c r="I1561">
-        <v>329.69429380908326</v>
-      </c>
-    </row>
-    <row r="1562" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1562" t="s">
+      <c r="Y1613">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1614" t="s">
         <v>36</v>
       </c>
-      <c r="B1562" s="1">
+      <c r="B1614" s="1">
         <v>45604</v>
       </c>
-      <c r="D1562">
-        <v>408.88193953844853</v>
-      </c>
-      <c r="E1562">
-        <v>1776.710706619858</v>
-      </c>
-      <c r="F1562">
-        <v>102.95759727412306</v>
-      </c>
-      <c r="I1562">
-        <v>374.82335583862925</v>
-      </c>
-    </row>
-    <row r="1563" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1563" t="s">
+      <c r="Y1614">
+        <v>5.958333333333333</v>
+      </c>
+    </row>
+    <row r="1615" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1615" t="s">
         <v>36</v>
       </c>
-      <c r="B1563" s="1">
+      <c r="B1615" s="1">
         <v>45610</v>
       </c>
-      <c r="D1563">
-        <v>338.10726437090386</v>
-      </c>
-      <c r="E1563">
-        <v>2056.7109163546615</v>
-      </c>
-      <c r="F1563">
-        <v>127.76178655901568</v>
-      </c>
-      <c r="I1563">
-        <v>474.46898821776767</v>
-      </c>
-    </row>
-    <row r="1564" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1564" t="s">
+      <c r="Y1615">
+        <v>6.2291666666666661</v>
+      </c>
+    </row>
+    <row r="1616" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1616" t="s">
         <v>36</v>
       </c>
-      <c r="B1564" s="1">
+      <c r="B1616" s="1">
         <v>45618</v>
       </c>
-      <c r="D1564">
-        <v>373.13635477443734</v>
-      </c>
-      <c r="E1564">
-        <v>2082.3687585393864</v>
-      </c>
-      <c r="F1564">
-        <v>104.71738647306412</v>
-      </c>
-      <c r="I1564">
-        <v>691.00767781564412</v>
-      </c>
-    </row>
-    <row r="1565" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1565" t="s">
+      <c r="Y1616">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1617" t="s">
         <v>36</v>
       </c>
-      <c r="B1565" s="1">
+      <c r="B1617" s="1">
         <v>45625</v>
       </c>
-      <c r="D1565">
-        <v>316.75768574125851</v>
-      </c>
-      <c r="E1565">
-        <v>2145.4009574182942</v>
-      </c>
-      <c r="F1565">
-        <v>189.98158021266462</v>
-      </c>
-      <c r="I1565">
-        <v>1130.1191945026715</v>
-      </c>
-    </row>
-    <row r="1566" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1566" t="s">
+      <c r="Y1617">
+        <v>5.833333333333333</v>
+      </c>
+    </row>
+    <row r="1618" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1618" t="s">
         <v>36</v>
       </c>
-      <c r="B1566" s="1">
+      <c r="B1618" s="1">
         <v>45631</v>
       </c>
-      <c r="D1566">
-        <v>294.11281369955356</v>
-      </c>
-      <c r="E1566">
-        <v>2041.2841052921665</v>
-      </c>
-      <c r="F1566">
-        <v>181.23353208103296</v>
-      </c>
-      <c r="I1566">
-        <v>1514.4728834719642</v>
-      </c>
-    </row>
-    <row r="1567" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1567" t="s">
+      <c r="Y1618">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="1619" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1619" t="s">
         <v>36</v>
       </c>
-      <c r="B1567" s="1">
+      <c r="B1619" s="1">
         <v>45637</v>
       </c>
-      <c r="D1567">
-        <v>258.28823302104024</v>
-      </c>
-      <c r="E1567">
-        <v>1827.4344542916051</v>
-      </c>
-      <c r="F1567">
-        <v>227.7889565165284</v>
-      </c>
-      <c r="I1567">
-        <v>1895.3564896875487</v>
-      </c>
-    </row>
-    <row r="1568" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1568" t="s">
+      <c r="Y1619">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="1620" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1620" t="s">
         <v>36</v>
       </c>
-      <c r="B1568" s="1">
+      <c r="B1620" s="1">
         <v>45644</v>
       </c>
-      <c r="D1568">
-        <v>220.72429200967147</v>
-      </c>
-      <c r="E1568">
-        <v>1549.7556732010034</v>
-      </c>
-      <c r="F1568">
-        <v>201.22701023133186</v>
-      </c>
-      <c r="I1568">
-        <v>2451.277432217395</v>
-      </c>
-    </row>
-    <row r="1569" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1569" t="s">
+      <c r="Y1620">
+        <v>4.6666666666666661</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1621" t="s">
         <v>36</v>
       </c>
-      <c r="B1569" s="1">
+      <c r="B1621" s="1">
         <v>45650</v>
       </c>
-      <c r="D1569">
-        <v>91.043943931492464</v>
-      </c>
-      <c r="E1569">
-        <v>1390.3038194136948</v>
-      </c>
-      <c r="F1569">
-        <v>300.67488131047168</v>
-      </c>
-      <c r="I1569">
-        <v>2675.9253562720319</v>
-      </c>
-    </row>
-    <row r="1570" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1570" t="s">
+      <c r="Y1621">
+        <v>4.916666666666667</v>
+      </c>
+    </row>
+    <row r="1622" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1622" t="s">
         <v>36</v>
       </c>
-      <c r="B1570" s="1">
+      <c r="B1622" s="1">
         <v>45656</v>
       </c>
-      <c r="D1570">
-        <v>61.988216464843276</v>
-      </c>
-      <c r="E1570">
-        <v>1288.0779880136479</v>
-      </c>
-      <c r="F1570">
-        <v>327.61268603122437</v>
-      </c>
-      <c r="I1570">
-        <v>2909.0410933907701</v>
-      </c>
-    </row>
-    <row r="1571" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1571" t="s">
+      <c r="Y1622">
+        <v>4.666666666666667</v>
+      </c>
+    </row>
+    <row r="1623" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1623" t="s">
         <v>36</v>
       </c>
-      <c r="B1571" s="1">
+      <c r="B1623" s="1">
         <v>45663</v>
       </c>
-      <c r="D1571">
-        <v>16.678329944359628</v>
-      </c>
-      <c r="E1571">
-        <v>1193.6529923653559</v>
-      </c>
-      <c r="F1571">
-        <v>317.04178865183826</v>
-      </c>
-      <c r="I1571">
-        <v>2486.9908485024071</v>
-      </c>
-    </row>
-    <row r="1572" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1572" t="s">
+      <c r="Y1623">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1624" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1624" t="s">
         <v>34</v>
       </c>
-      <c r="B1572" s="1">
+      <c r="B1624" s="1">
+        <v>45443</v>
+      </c>
+      <c r="Y1624">
+        <v>8.8333333333333321</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1625" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1625" s="1">
+        <v>45449</v>
+      </c>
+      <c r="Y1625">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1626" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1626" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1626" s="1">
+        <v>45456</v>
+      </c>
+      <c r="Y1626">
+        <v>14.666666666666668</v>
+      </c>
+    </row>
+    <row r="1627" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1627" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1627" s="1">
+        <v>45462</v>
+      </c>
+      <c r="Y1627">
+        <v>19.833333333333336</v>
+      </c>
+    </row>
+    <row r="1628" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1628" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1628" s="1">
+        <v>45469</v>
+      </c>
+      <c r="Y1628">
+        <v>12.666666666666668</v>
+      </c>
+    </row>
+    <row r="1629" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1629" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1629" s="1">
+        <v>45477</v>
+      </c>
+      <c r="Y1629">
+        <v>17.833333333333336</v>
+      </c>
+    </row>
+    <row r="1630" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1630" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1630" s="1">
+        <v>45483</v>
+      </c>
+      <c r="Y1630">
+        <v>14.333333333333334</v>
+      </c>
+    </row>
+    <row r="1631" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1631" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1631" s="1">
+        <v>45492</v>
+      </c>
+      <c r="Y1631">
+        <v>15.666666666666668</v>
+      </c>
+    </row>
+    <row r="1632" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1632" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1632" s="1">
+        <v>45500</v>
+      </c>
+      <c r="Y1632">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="1633" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1633" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1633" s="1">
+        <v>45505</v>
+      </c>
+      <c r="Y1633">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1634" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1634" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1634" s="1">
+        <v>45512</v>
+      </c>
+      <c r="Y1634">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1635" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1635" s="1">
+        <v>45520</v>
+      </c>
+      <c r="Y1635">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1636" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1636" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1636" s="1">
+        <v>45527</v>
+      </c>
+      <c r="Y1636">
+        <v>16.166666666666668</v>
+      </c>
+    </row>
+    <row r="1637" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1637" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1637" s="1">
+        <v>45533</v>
+      </c>
+      <c r="Y1637">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1638" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1638" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1638" s="1">
+        <v>45539</v>
+      </c>
+      <c r="Y1638">
+        <v>12.333333333333334</v>
+      </c>
+    </row>
+    <row r="1639" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1639" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1639" s="1">
+        <v>45545</v>
+      </c>
+      <c r="Y1639">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1640" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1640" s="1">
+        <v>45555</v>
+      </c>
+      <c r="Y1640">
+        <v>9.6666666666666661</v>
+      </c>
+    </row>
+    <row r="1641" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1641" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1641" s="1">
+        <v>45562</v>
+      </c>
+      <c r="Y1641">
+        <v>10.833333333333332</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1642" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1642" s="1">
+        <v>45569</v>
+      </c>
+      <c r="Y1642">
+        <v>8.3333333333333321</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1643" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1643" s="1">
+        <v>45575</v>
+      </c>
+      <c r="Y1643">
+        <v>10.333333333333332</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1644" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1644" s="1">
+        <v>45581</v>
+      </c>
+      <c r="Y1644">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1645" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1645" s="1">
+        <v>45590</v>
+      </c>
+      <c r="Y1645">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1646" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1646" s="1">
         <v>45597</v>
       </c>
-      <c r="D1572">
-        <v>415.22016874701114</v>
-      </c>
-      <c r="E1572">
-        <v>1600.385730890262</v>
-      </c>
-      <c r="F1572">
-        <v>132.98844733685718</v>
-      </c>
-      <c r="I1572">
-        <v>277.42532970992147</v>
-      </c>
-    </row>
-    <row r="1573" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1573" t="s">
+      <c r="Y1646">
+        <v>7.604166666666667</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1647" t="s">
         <v>34</v>
       </c>
-      <c r="B1573" s="1">
+      <c r="B1647" s="1">
         <v>45604</v>
       </c>
-      <c r="D1573">
-        <v>446.67035476974218</v>
-      </c>
-      <c r="E1573">
-        <v>1769.1736306968644</v>
-      </c>
-      <c r="F1573">
-        <v>152.22275917420157</v>
-      </c>
-      <c r="I1573">
-        <v>397.820234643189</v>
-      </c>
-    </row>
-    <row r="1574" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1574" t="s">
+      <c r="Y1647">
+        <v>6.833333333333333</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1648" t="s">
         <v>34</v>
       </c>
-      <c r="B1574" s="1">
+      <c r="B1648" s="1">
         <v>45610</v>
       </c>
-      <c r="D1574">
-        <v>426.3562140813932</v>
-      </c>
-      <c r="E1574">
-        <v>1695.1513781097215</v>
-      </c>
-      <c r="F1574">
-        <v>102.50855144462201</v>
-      </c>
-      <c r="I1574">
-        <v>439.69822603225236</v>
-      </c>
-    </row>
-    <row r="1575" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1575" t="s">
+      <c r="Y1648">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1649" t="s">
         <v>34</v>
       </c>
-      <c r="B1575" s="1">
+      <c r="B1649" s="1">
         <v>45618</v>
       </c>
-      <c r="D1575">
-        <v>393.47926553917034</v>
-      </c>
-      <c r="E1575">
-        <v>1979.801940795033</v>
-      </c>
-      <c r="F1575">
-        <v>157.69280794493309</v>
-      </c>
-      <c r="I1575">
-        <v>733.76253763854754</v>
-      </c>
-    </row>
-    <row r="1576" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1576" t="s">
+      <c r="Y1649">
+        <v>5.5833333333333339</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1650" t="s">
         <v>34</v>
       </c>
-      <c r="B1576" s="1">
+      <c r="B1650" s="1">
         <v>45625</v>
       </c>
-      <c r="D1576">
-        <v>438.17891064379398</v>
-      </c>
-      <c r="E1576">
-        <v>2215.361621881571</v>
-      </c>
-      <c r="F1576">
-        <v>150.57108174240977</v>
-      </c>
-      <c r="I1576">
-        <v>1189.4543229336527</v>
-      </c>
-    </row>
-    <row r="1577" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1577" t="s">
+      <c r="Y1650">
+        <v>6.333333333333333</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1651" t="s">
         <v>34</v>
       </c>
-      <c r="B1577" s="1">
+      <c r="B1651" s="1">
         <v>45631</v>
       </c>
-      <c r="D1577">
-        <v>446.11715325474518</v>
-      </c>
-      <c r="E1577">
-        <v>2246.572820744213</v>
-      </c>
-      <c r="F1577">
-        <v>171.02298734068302</v>
-      </c>
-      <c r="I1577">
-        <v>1639.9361318887552</v>
-      </c>
-    </row>
-    <row r="1578" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1578" t="s">
+      <c r="Y1651">
+        <v>5.8749999999999991</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1652" t="s">
         <v>34</v>
       </c>
-      <c r="B1578" s="1">
+      <c r="B1652" s="1">
         <v>45637</v>
       </c>
-      <c r="D1578">
-        <v>309.45394979689769</v>
-      </c>
-      <c r="E1578">
-        <v>1889.405858311271</v>
-      </c>
-      <c r="F1578">
-        <v>210.89403009268602</v>
-      </c>
-      <c r="I1578">
-        <v>1954.0972950304247</v>
-      </c>
-    </row>
-    <row r="1579" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1579" t="s">
+      <c r="Y1652">
+        <v>5.833333333333333</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1653" t="s">
         <v>34</v>
       </c>
-      <c r="B1579" s="1">
+      <c r="B1653" s="1">
         <v>45644</v>
       </c>
-      <c r="D1579">
-        <v>266.07289423895742</v>
-      </c>
-      <c r="E1579">
-        <v>1554.5976625938974</v>
-      </c>
-      <c r="F1579">
-        <v>247.24567850519992</v>
-      </c>
-      <c r="I1579">
-        <v>2333.9275296536803</v>
-      </c>
-    </row>
-    <row r="1580" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1580" t="s">
+      <c r="Y1653">
+        <v>5.833333333333333</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1654" t="s">
         <v>34</v>
       </c>
-      <c r="B1580" s="1">
+      <c r="B1654" s="1">
         <v>45650</v>
       </c>
-      <c r="D1580">
-        <v>102.73555771562553</v>
-      </c>
-      <c r="E1580">
-        <v>1577.883375463912</v>
-      </c>
-      <c r="F1580">
-        <v>345.74726369035983</v>
-      </c>
-      <c r="I1580">
-        <v>3035.3261120304801</v>
-      </c>
-    </row>
-    <row r="1581" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1581" t="s">
+      <c r="Y1654">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1655" t="s">
         <v>34</v>
       </c>
-      <c r="B1581" s="1">
+      <c r="B1655" s="1">
         <v>45656</v>
       </c>
-      <c r="D1581">
-        <v>88.431849729217817</v>
-      </c>
-      <c r="E1581">
-        <v>1445.8538223815892</v>
-      </c>
-      <c r="F1581">
-        <v>339.20551859734059</v>
-      </c>
-      <c r="I1581">
-        <v>3255.4777084854377</v>
-      </c>
-    </row>
-    <row r="1582" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1582" t="s">
+      <c r="Y1655">
+        <v>5.416666666666667</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1656" t="s">
         <v>34</v>
       </c>
-      <c r="B1582" s="1">
+      <c r="B1656" s="1">
         <v>45663</v>
       </c>
-      <c r="D1582">
-        <v>0</v>
-      </c>
-      <c r="E1582">
-        <v>1398.3231445323981</v>
-      </c>
-      <c r="F1582">
-        <v>354.499341548953</v>
-      </c>
-      <c r="I1582">
-        <v>2798.0237715363896</v>
-      </c>
-    </row>
-    <row r="1583" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1583" t="s">
+      <c r="Y1656">
+        <v>5.4166666666666661</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1657" t="s">
         <v>35</v>
       </c>
-      <c r="B1583" s="1">
+      <c r="B1657" s="1">
+        <v>45443</v>
+      </c>
+      <c r="Y1657">
+        <v>13.666666666666668</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1658" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1658" s="1">
+        <v>45449</v>
+      </c>
+      <c r="Y1658">
+        <v>14.833333333333334</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1659" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1659" s="1">
+        <v>45456</v>
+      </c>
+      <c r="Y1659">
+        <v>12.833333333333334</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1660" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1660" s="1">
+        <v>45462</v>
+      </c>
+      <c r="Y1660">
+        <v>15.333333333333332</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1661" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1661" s="1">
+        <v>45469</v>
+      </c>
+      <c r="Y1661">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1662" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1662" s="1">
+        <v>45477</v>
+      </c>
+      <c r="Y1662">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1663" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1663" s="1">
+        <v>45483</v>
+      </c>
+      <c r="Y1663">
+        <v>13.333333333333332</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1664" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1664" s="1">
+        <v>45492</v>
+      </c>
+      <c r="Y1664">
+        <v>16.333333333333332</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1665" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1665" s="1">
+        <v>45500</v>
+      </c>
+      <c r="Y1665">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1666" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1666" s="1">
+        <v>45505</v>
+      </c>
+      <c r="Y1666">
+        <v>15.166666666666666</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1667" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1667" s="1">
+        <v>45512</v>
+      </c>
+      <c r="Y1667">
+        <v>12.833333333333332</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1668" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1668" s="1">
+        <v>45520</v>
+      </c>
+      <c r="Y1668">
+        <v>16.333333333333336</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1669" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1669" s="1">
+        <v>45527</v>
+      </c>
+      <c r="Y1669">
+        <v>15.666666666666666</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1670" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1670" s="1">
+        <v>45533</v>
+      </c>
+      <c r="Y1670">
+        <v>15.25</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1671" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1671" s="1">
+        <v>45539</v>
+      </c>
+      <c r="Y1671">
+        <v>14.666666666666668</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1672" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1672" s="1">
+        <v>45545</v>
+      </c>
+      <c r="Y1672">
+        <v>14.083333333333332</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1673" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1673" s="1">
+        <v>45555</v>
+      </c>
+      <c r="Y1673">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1674" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1674" s="1">
+        <v>45562</v>
+      </c>
+      <c r="Y1674">
+        <v>12.416666666666668</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1675" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1675" s="1">
+        <v>45569</v>
+      </c>
+      <c r="Y1675">
+        <v>12.333333333333332</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1676" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1676" s="1">
+        <v>45575</v>
+      </c>
+      <c r="Y1676">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1677" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1677" s="1">
+        <v>45581</v>
+      </c>
+      <c r="Y1677">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1678" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1678" s="1">
+        <v>45590</v>
+      </c>
+      <c r="Y1678">
+        <v>7.666666666666667</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1679" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1679" s="1">
         <v>45597</v>
       </c>
-      <c r="D1583">
-        <v>494.40043935304925</v>
-      </c>
-      <c r="E1583">
-        <v>1693.6091392008793</v>
-      </c>
-      <c r="F1583">
-        <v>86.864936950205049</v>
-      </c>
-      <c r="I1583">
-        <v>356.6092829408928</v>
-      </c>
-    </row>
-    <row r="1584" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1584" t="s">
+      <c r="Y1679">
+        <v>6.4999999999999991</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1680" t="s">
         <v>35</v>
       </c>
-      <c r="B1584" s="1">
+      <c r="B1680" s="1">
         <v>45604</v>
       </c>
-      <c r="D1584">
-        <v>503.62896006171928</v>
-      </c>
-      <c r="E1584">
-        <v>1910.8711873026075</v>
-      </c>
-      <c r="F1584">
-        <v>111.64829048218641</v>
-      </c>
-      <c r="I1584">
-        <v>450.13517961230821</v>
-      </c>
-    </row>
-    <row r="1585" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1585" t="s">
+      <c r="Y1680">
+        <v>7.4166666666666679</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1681" t="s">
         <v>35</v>
       </c>
-      <c r="B1585" s="1">
+      <c r="B1681" s="1">
         <v>45610</v>
       </c>
-      <c r="D1585">
-        <v>500.85046265495754</v>
-      </c>
-      <c r="E1585">
-        <v>2107.6276434466245</v>
-      </c>
-      <c r="F1585">
-        <v>117.2187949004025</v>
-      </c>
-      <c r="I1585">
-        <v>552.17583026562102</v>
-      </c>
-    </row>
-    <row r="1586" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1586" t="s">
+      <c r="Y1681">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1682" t="s">
         <v>35</v>
       </c>
-      <c r="B1586" s="1">
+      <c r="B1682" s="1">
         <v>45618</v>
       </c>
-      <c r="D1586">
-        <v>426.65396343069091</v>
-      </c>
-      <c r="E1586">
-        <v>2092.8185613616679</v>
-      </c>
-      <c r="F1586">
-        <v>140.95655355875937</v>
-      </c>
-      <c r="I1586">
-        <v>788.24226538281823</v>
-      </c>
-    </row>
-    <row r="1587" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1587" t="s">
+      <c r="Y1682">
+        <v>6.9999999999999991</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1683" t="s">
         <v>35</v>
       </c>
-      <c r="B1587" s="1">
+      <c r="B1683" s="1">
         <v>45625</v>
       </c>
-      <c r="D1587">
-        <v>450.21651520831301</v>
-      </c>
-      <c r="E1587">
-        <v>2210.4525326468183</v>
-      </c>
-      <c r="F1587">
-        <v>179.8960162650242</v>
-      </c>
-      <c r="I1587">
-        <v>1202.80589909276</v>
-      </c>
-    </row>
-    <row r="1588" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1588" t="s">
+      <c r="Y1683">
+        <v>7.1666666666666679</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1684" t="s">
         <v>35</v>
       </c>
-      <c r="B1588" s="1">
+      <c r="B1684" s="1">
         <v>45631</v>
       </c>
-      <c r="D1588">
-        <v>409.95245869881114</v>
-      </c>
-      <c r="E1588">
-        <v>2181.5429988675255</v>
-      </c>
-      <c r="F1588">
-        <v>191.18178753622394</v>
-      </c>
-      <c r="I1588">
-        <v>1704.7244335422038</v>
-      </c>
-    </row>
-    <row r="1589" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1589" t="s">
+      <c r="Y1684">
+        <v>6.4166666666666661</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1685" t="s">
         <v>35</v>
       </c>
-      <c r="B1589" s="1">
+      <c r="B1685" s="1">
         <v>45637</v>
       </c>
-      <c r="D1589">
-        <v>314.65142427886246</v>
-      </c>
-      <c r="E1589">
-        <v>1787.5591050714811</v>
-      </c>
-      <c r="F1589">
-        <v>227.06282818460437</v>
-      </c>
-      <c r="I1589">
-        <v>1995.0810911222779</v>
-      </c>
-    </row>
-    <row r="1590" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1590" t="s">
+      <c r="Y1685">
+        <v>6.166666666666667</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1686" t="s">
         <v>35</v>
       </c>
-      <c r="B1590" s="1">
+      <c r="B1686" s="1">
         <v>45644</v>
       </c>
-      <c r="D1590">
-        <v>261.38595695602095</v>
-      </c>
-      <c r="E1590">
-        <v>1560.2297313442755</v>
-      </c>
-      <c r="F1590">
-        <v>243.68975700023415</v>
-      </c>
-      <c r="I1590">
-        <v>2517.440328998674</v>
-      </c>
-    </row>
-    <row r="1591" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1591" t="s">
+      <c r="Y1686">
+        <v>6.416666666666667</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1687" t="s">
         <v>35</v>
       </c>
-      <c r="B1591" s="1">
+      <c r="B1687" s="1">
         <v>45650</v>
       </c>
-      <c r="D1591">
-        <v>264.71586785552631</v>
-      </c>
-      <c r="E1591">
-        <v>1567.7022895058094</v>
-      </c>
-      <c r="F1591">
-        <v>241.70789629313876</v>
-      </c>
-      <c r="I1591">
-        <v>3000.1469757147506</v>
-      </c>
-    </row>
-    <row r="1592" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1592" t="s">
+      <c r="Y1687">
+        <v>5.583333333333333</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1688" t="s">
         <v>35</v>
       </c>
-      <c r="B1592" s="1">
+      <c r="B1688" s="1">
         <v>45656</v>
       </c>
-      <c r="D1592">
-        <v>67.252714674168999</v>
-      </c>
-      <c r="E1592">
-        <v>1494.7710088968145</v>
-      </c>
-      <c r="F1592">
-        <v>377.82888366675627</v>
-      </c>
-      <c r="I1592">
-        <v>3198.991507884336</v>
-      </c>
-    </row>
-    <row r="1593" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1593" t="s">
+      <c r="Y1688">
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1689" t="s">
         <v>35</v>
       </c>
-      <c r="B1593" s="1">
+      <c r="B1689" s="1">
         <v>45663</v>
       </c>
-      <c r="D1593">
-        <v>20.807004426980797</v>
-      </c>
-      <c r="E1593">
-        <v>1355.9054761598836</v>
-      </c>
-      <c r="F1593">
-        <v>370.5811826661656</v>
-      </c>
-      <c r="I1593">
-        <v>2785.8836981060431</v>
+      <c r="Y1689">
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1690" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1690" s="1">
+        <v>45456</v>
+      </c>
+      <c r="Y1690">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1691" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1691" s="1">
+        <v>45462</v>
+      </c>
+      <c r="Y1691">
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1692" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1692" s="1">
+        <v>45469</v>
+      </c>
+      <c r="Y1692">
+        <v>3.1111111111111107</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1693" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1693" s="1">
+        <v>45477</v>
+      </c>
+      <c r="Y1693">
+        <v>4.666666666666667</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1694" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1694" s="1">
+        <v>45483</v>
+      </c>
+      <c r="Y1694">
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1695" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1695" s="1">
+        <v>45492</v>
+      </c>
+      <c r="Y1695">
+        <v>6.8333333333333339</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1696" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1696" s="1">
+        <v>45500</v>
+      </c>
+      <c r="Y1696">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1697" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1697" s="1">
+        <v>45505</v>
+      </c>
+      <c r="Y1697">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1698" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1698" s="1">
+        <v>45512</v>
+      </c>
+      <c r="Y1698">
+        <v>10.833333333333332</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1699" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1699" s="1">
+        <v>45520</v>
+      </c>
+      <c r="Y1699">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1700" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1700" s="1">
+        <v>45527</v>
+      </c>
+      <c r="Y1700">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1701" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1701" s="1">
+        <v>45533</v>
+      </c>
+      <c r="Y1701">
+        <v>14.833333333333332</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1702" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1702" s="1">
+        <v>45539</v>
+      </c>
+      <c r="Y1702">
+        <v>12.666666666666668</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1703" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1703" s="1">
+        <v>45546</v>
+      </c>
+      <c r="Y1703">
+        <v>9.1666666666666661</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1704" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1704" s="1">
+        <v>45555</v>
+      </c>
+      <c r="Y1704">
+        <v>9.8333333333333321</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1705" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1705" s="1">
+        <v>45562</v>
+      </c>
+      <c r="Y1705">
+        <v>8.8333333333333321</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1706" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1706" s="1">
+        <v>45569</v>
+      </c>
+      <c r="Y1706">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1707" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1707" s="1">
+        <v>45575</v>
+      </c>
+      <c r="Y1707">
+        <v>8.6666666666666661</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1708" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1708" s="1">
+        <v>45581</v>
+      </c>
+      <c r="Y1708">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1709" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1709" s="1">
+        <v>45590</v>
+      </c>
+      <c r="Y1709">
+        <v>7.6666666666666661</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1710" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1710" s="1">
+        <v>45597</v>
+      </c>
+      <c r="Y1710">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1711" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1711" s="1">
+        <v>45604</v>
+      </c>
+      <c r="Y1711">
+        <v>6.854166666666667</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1712" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1712" s="1">
+        <v>45610</v>
+      </c>
+      <c r="Y1712">
+        <v>6.0833333333333339</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1713" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1713" s="1">
+        <v>45618</v>
+      </c>
+      <c r="Y1713">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1714" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1714" s="1">
+        <v>45625</v>
+      </c>
+      <c r="Y1714">
+        <v>6.4999999999999991</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1715" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1715" s="1">
+        <v>45631</v>
+      </c>
+      <c r="Y1715">
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1716" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1716" s="1">
+        <v>45637</v>
+      </c>
+      <c r="Y1716">
+        <v>4.833333333333333</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1717" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1717" s="1">
+        <v>45644</v>
+      </c>
+      <c r="Y1717">
+        <v>4.583333333333333</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1718" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1718" s="1">
+        <v>45650</v>
+      </c>
+      <c r="Y1718">
+        <v>4.916666666666667</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1719" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1719" s="1">
+        <v>45656</v>
+      </c>
+      <c r="Y1719">
+        <v>5.5833333333333339</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1720" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1720" s="1">
+        <v>45663</v>
+      </c>
+      <c r="Y1720">
+        <v>4.833333333333333</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1721" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1721" s="1">
+        <v>45669</v>
+      </c>
+      <c r="Y1721">
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1722" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1722" s="1">
+        <v>45674</v>
+      </c>
+      <c r="Y1722">
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1723" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1723" s="1">
+        <v>45456</v>
+      </c>
+      <c r="Y1723">
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1724" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1724" s="1">
+        <v>45462</v>
+      </c>
+      <c r="Y1724">
+        <v>3.2222222222222228</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1725" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1725" s="1">
+        <v>45469</v>
+      </c>
+      <c r="Y1725">
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1726" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1726" s="1">
+        <v>45477</v>
+      </c>
+      <c r="Y1726">
+        <v>4.1111111111111116</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1727" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1727" s="1">
+        <v>45483</v>
+      </c>
+      <c r="Y1727">
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1728" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1728" s="1">
+        <v>45492</v>
+      </c>
+      <c r="Y1728">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1729" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1729" s="1">
+        <v>45500</v>
+      </c>
+      <c r="Y1729">
+        <v>5.166666666666667</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1730" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1730" s="1">
+        <v>45505</v>
+      </c>
+      <c r="Y1730">
+        <v>9.8333333333333321</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1731" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1731" s="1">
+        <v>45512</v>
+      </c>
+      <c r="Y1731">
+        <v>7.8333333333333339</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1732" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1732" s="1">
+        <v>45520</v>
+      </c>
+      <c r="Y1732">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1733" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1733" s="1">
+        <v>45527</v>
+      </c>
+      <c r="Y1733">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1734" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1734" s="1">
+        <v>45533</v>
+      </c>
+      <c r="Y1734">
+        <v>9.1666666666666661</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1735" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1735" s="1">
+        <v>45539</v>
+      </c>
+      <c r="Y1735">
+        <v>14.166666666666668</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1736" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1736" s="1">
+        <v>45546</v>
+      </c>
+      <c r="Y1736">
+        <v>10.166666666666666</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1737" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1737" s="1">
+        <v>45555</v>
+      </c>
+      <c r="Y1737">
+        <v>9.3333333333333339</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1738" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1738" s="1">
+        <v>45562</v>
+      </c>
+      <c r="Y1738">
+        <v>11.583333333333332</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1739" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1739" s="1">
+        <v>45569</v>
+      </c>
+      <c r="Y1739">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1740" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1740" s="1">
+        <v>45575</v>
+      </c>
+      <c r="Y1740">
+        <v>10.666666666666666</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1741" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1741" s="1">
+        <v>45581</v>
+      </c>
+      <c r="Y1741">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1742" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1742" s="1">
+        <v>45590</v>
+      </c>
+      <c r="Y1742">
+        <v>7.8333333333333339</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1743" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1743" s="1">
+        <v>45597</v>
+      </c>
+      <c r="Y1743">
+        <v>7.166666666666667</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1744" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1744" s="1">
+        <v>45604</v>
+      </c>
+      <c r="Y1744">
+        <v>7.6875</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1745" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1745" s="1">
+        <v>45610</v>
+      </c>
+      <c r="Y1745">
+        <v>7.083333333333333</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1746" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1746" s="1">
+        <v>45618</v>
+      </c>
+      <c r="Y1746">
+        <v>6.4166666666666661</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1747" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1747" s="1">
+        <v>45625</v>
+      </c>
+      <c r="Y1747">
+        <v>6.5000000000000009</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1748" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1748" s="1">
+        <v>45631</v>
+      </c>
+      <c r="Y1748">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1749" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1749" s="1">
+        <v>45637</v>
+      </c>
+      <c r="Y1749">
+        <v>5.583333333333333</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1750" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1750" s="1">
+        <v>45644</v>
+      </c>
+      <c r="Y1750">
+        <v>5.4166666666666661</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1751" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1751" s="1">
+        <v>45650</v>
+      </c>
+      <c r="Y1751">
+        <v>5.2222222222222223</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1752" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1752" s="1">
+        <v>45656</v>
+      </c>
+      <c r="Y1752">
+        <v>5.583333333333333</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1753" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1753" s="1">
+        <v>45663</v>
+      </c>
+      <c r="Y1753">
+        <v>5.5833333333333339</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1754" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1754" s="1">
+        <v>45669</v>
+      </c>
+      <c r="Y1754">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1755" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1755" s="1">
+        <v>45674</v>
+      </c>
+      <c r="Y1755">
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1756" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1756" s="1">
+        <v>45456</v>
+      </c>
+      <c r="Y1756">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1757" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1757" s="1">
+        <v>45462</v>
+      </c>
+      <c r="Y1757">
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1758" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1758" s="1">
+        <v>45469</v>
+      </c>
+      <c r="Y1758">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1759" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1759" s="1">
+        <v>45477</v>
+      </c>
+      <c r="Y1759">
+        <v>5.8333333333333339</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1760" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1760" s="1">
+        <v>45483</v>
+      </c>
+      <c r="Y1760">
+        <v>5.6666666666666661</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1761" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1761" s="1">
+        <v>45492</v>
+      </c>
+      <c r="Y1761">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1762" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1762" s="1">
+        <v>45500</v>
+      </c>
+      <c r="Y1762">
+        <v>6.3333333333333339</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1763" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1763" s="1">
+        <v>45505</v>
+      </c>
+      <c r="Y1763">
+        <v>7.6666666666666661</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1764" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1764" s="1">
+        <v>45512</v>
+      </c>
+      <c r="Y1764">
+        <v>12.166666666666666</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1765" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1765" s="1">
+        <v>45520</v>
+      </c>
+      <c r="Y1765">
+        <v>10.166666666666668</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1766" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1766" s="1">
+        <v>45527</v>
+      </c>
+      <c r="Y1766">
+        <v>11.666666666666668</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1767" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1767" s="1">
+        <v>45533</v>
+      </c>
+      <c r="Y1767">
+        <v>12.166666666666666</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1768" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1768" s="1">
+        <v>45539</v>
+      </c>
+      <c r="Y1768">
+        <v>12.666666666666668</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1769" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1769" s="1">
+        <v>45546</v>
+      </c>
+      <c r="Y1769">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1770" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1770" s="1">
+        <v>45555</v>
+      </c>
+      <c r="Y1770">
+        <v>10.166666666666668</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1771" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1771" s="1">
+        <v>45562</v>
+      </c>
+      <c r="Y1771">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1772" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1772" s="1">
+        <v>45569</v>
+      </c>
+      <c r="Y1772">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1773" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1773" s="1">
+        <v>45575</v>
+      </c>
+      <c r="Y1773">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1774" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1774" s="1">
+        <v>45581</v>
+      </c>
+      <c r="Y1774">
+        <v>8.6666666666666661</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1775" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1775" s="1">
+        <v>45590</v>
+      </c>
+      <c r="Y1775">
+        <v>7.1666666666666661</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1776" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1776" s="1">
+        <v>45597</v>
+      </c>
+      <c r="Y1776">
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1777" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1777" s="1">
+        <v>45604</v>
+      </c>
+      <c r="Y1777">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1778" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1778" s="1">
+        <v>45610</v>
+      </c>
+      <c r="Y1778">
+        <v>6.3333333333333339</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1779" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1779" s="1">
+        <v>45618</v>
+      </c>
+      <c r="Y1779">
+        <v>6.416666666666667</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1780" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1780" s="1">
+        <v>45625</v>
+      </c>
+      <c r="Y1780">
+        <v>7.104166666666667</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1781" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1781" s="1">
+        <v>45631</v>
+      </c>
+      <c r="Y1781">
+        <v>6.8333333333333339</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1782" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1782" s="1">
+        <v>45637</v>
+      </c>
+      <c r="Y1782">
+        <v>5.916666666666667</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1783" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1783" s="1">
+        <v>45644</v>
+      </c>
+      <c r="Y1783">
+        <v>5.583333333333333</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1784" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1784" s="1">
+        <v>45650</v>
+      </c>
+      <c r="Y1784">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1785" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1785" s="1">
+        <v>45656</v>
+      </c>
+      <c r="Y1785">
+        <v>5.416666666666667</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1786" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1786" s="1">
+        <v>45663</v>
+      </c>
+      <c r="Y1786">
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1787" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1787" s="1">
+        <v>45669</v>
+      </c>
+      <c r="Y1787">
+        <v>5.4166666666666661</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1788" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1788" s="1">
+        <v>45674</v>
+      </c>
+      <c r="Y1788">
+        <v>6.166666666666667</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1789" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1789" s="1">
+        <v>45456</v>
+      </c>
+      <c r="Y1789">
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1790" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1790" s="1">
+        <v>45462</v>
+      </c>
+      <c r="Y1790">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1791" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1791" s="1">
+        <v>45469</v>
+      </c>
+      <c r="Y1791">
+        <v>2.8333333333333335</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1792" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1792" s="1">
+        <v>45477</v>
+      </c>
+      <c r="Y1792">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1793" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1793" s="1">
+        <v>45483</v>
+      </c>
+      <c r="Y1793">
+        <v>3.8333333333333335</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1794" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1794" s="1">
+        <v>45492</v>
+      </c>
+      <c r="Y1794">
+        <v>5.833333333333333</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1795" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1795" s="1">
+        <v>45500</v>
+      </c>
+      <c r="Y1795">
+        <v>6.3333333333333339</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1796" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1796" s="1">
+        <v>45505</v>
+      </c>
+      <c r="Y1796">
+        <v>8.1666666666666661</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1797" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1797" s="1">
+        <v>45512</v>
+      </c>
+      <c r="Y1797">
+        <v>7.3333333333333339</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1798" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1798" s="1">
+        <v>45520</v>
+      </c>
+      <c r="Y1798">
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1799" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1799" s="1">
+        <v>45527</v>
+      </c>
+      <c r="Y1799">
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1800" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1800" s="1">
+        <v>45533</v>
+      </c>
+      <c r="Y1800">
+        <v>12.166666666666666</v>
+      </c>
+    </row>
+    <row r="1801" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1801" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1801" s="1">
+        <v>45539</v>
+      </c>
+      <c r="Y1801">
+        <v>10.833333333333332</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1802" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1802" s="1">
+        <v>45546</v>
+      </c>
+      <c r="Y1802">
+        <v>10.333333333333332</v>
+      </c>
+    </row>
+    <row r="1803" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1803" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1803" s="1">
+        <v>45555</v>
+      </c>
+      <c r="Y1803">
+        <v>9.6666666666666661</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1804" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1804" s="1">
+        <v>45562</v>
+      </c>
+      <c r="Y1804">
+        <v>9.3333333333333321</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1805" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1805" s="1">
+        <v>45569</v>
+      </c>
+      <c r="Y1805">
+        <v>8.6666666666666661</v>
+      </c>
+    </row>
+    <row r="1806" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1806" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1806" s="1">
+        <v>45575</v>
+      </c>
+      <c r="Y1806">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="1807" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1807" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1807" s="1">
+        <v>45581</v>
+      </c>
+      <c r="Y1807">
+        <v>9.3333333333333321</v>
+      </c>
+    </row>
+    <row r="1808" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1808" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1808" s="1">
+        <v>45590</v>
+      </c>
+      <c r="Y1808">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1809" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1809" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1809" s="1">
+        <v>45597</v>
+      </c>
+      <c r="Y1809">
+        <v>7.666666666666667</v>
+      </c>
+    </row>
+    <row r="1810" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1810" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1810" s="1">
+        <v>45604</v>
+      </c>
+      <c r="Y1810">
+        <v>7.729166666666667</v>
+      </c>
+    </row>
+    <row r="1811" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1811" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1811" s="1">
+        <v>45610</v>
+      </c>
+      <c r="Y1811">
+        <v>7.583333333333333</v>
+      </c>
+    </row>
+    <row r="1812" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1812" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1812" s="1">
+        <v>45618</v>
+      </c>
+      <c r="Y1812">
+        <v>6.4166666666666661</v>
+      </c>
+    </row>
+    <row r="1813" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1813" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1813" s="1">
+        <v>45625</v>
+      </c>
+      <c r="Y1813">
+        <v>6.958333333333333</v>
+      </c>
+    </row>
+    <row r="1814" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1814" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1814" s="1">
+        <v>45631</v>
+      </c>
+      <c r="Y1814">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="1815" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1815" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1815" s="1">
+        <v>45637</v>
+      </c>
+      <c r="Y1815">
+        <v>6.3333333333333339</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1816" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1816" s="1">
+        <v>45644</v>
+      </c>
+      <c r="Y1816">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="1817" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1817" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1817" s="1">
+        <v>45650</v>
+      </c>
+      <c r="Y1817">
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="1818" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1818" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1818" s="1">
+        <v>45656</v>
+      </c>
+      <c r="Y1818">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="1819" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1819" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1819" s="1">
+        <v>45663</v>
+      </c>
+      <c r="Y1819">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1820" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1820" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1820" s="1">
+        <v>45669</v>
+      </c>
+      <c r="Y1820">
+        <v>6.333333333333333</v>
+      </c>
+    </row>
+    <row r="1821" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1821" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1821" s="1">
+        <v>45674</v>
+      </c>
+      <c r="Y1821">
+        <v>5.3333333333333339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bring changes back lost by conflict resolve
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/data/Lincoln2024.xlsx
+++ b/Tests/Validation/Wheat/data/Lincoln2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95990E4-387C-42D5-B7CF-6D68FB62BF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67928D1-1D3F-438F-AF02-584C483CB072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" autoFilterDateGrouping="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3985" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3985" uniqueCount="111">
   <si>
     <t>SimulationName</t>
   </si>
@@ -400,6 +400,9 @@
   <si>
     <t>Wheat.Phenology.Zadok.Stage-NotModeled</t>
   </si>
+  <si>
+    <t>Spectral.NDVI</t>
+  </si>
 </sst>
 </file>
 
@@ -37330,7 +37333,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CDB945A4-1CBA-4E3B-AECB-2763496B12BB}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CDB945A4-1CBA-4E3B-AECB-2763496B12BB}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="42">
     <pivotField axis="axisRow" showAll="0">
@@ -37791,8 +37794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14BBE95E-A304-486E-A4C6-DD8F3EEFA3AF}">
   <dimension ref="A1:AP833"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37840,7 +37843,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -94464,15 +94467,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002CA9C2C83C87A7408E0099D61CB2C224" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ce516e8a7524994cf4149f9aaa4cac7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="322cff4d-e128-4275-8c17-01ea60ce9850" xmlns:ns4="7391035e-a561-4b14-b643-167d3e77bc43" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="449e7fc92384ad82c475872e96556466" ns3:_="" ns4:_="">
     <xsd:import namespace="322cff4d-e128-4275-8c17-01ea60ce9850"/>
@@ -94725,6 +94719,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3709C4F5-F4CD-4825-B22E-AD384DC6F7E6}">
   <ds:schemaRefs>
@@ -94743,14 +94746,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{565FE936-45C1-4267-BB01-0C6ECA531FFF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1EA98CE-4368-4F90-9C57-5CE2133AA34B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -94767,4 +94762,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{565FE936-45C1-4267-BB01-0C6ECA531FFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>